<commit_message>
enp y variables de incumbente
</commit_message>
<xml_diff>
--- a/output/231030 - Pactos.xlsx
+++ b/output/231030 - Pactos.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>PARTIDO REGIONALISTA INDEPENDIENTE</t>
+          <t>PARTIDO REGIONALISTA DE MAGALLANES</t>
         </is>
       </c>
     </row>
@@ -1955,12 +1955,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>RENOVACION NACIONAL</t>
+          <t>PODER</t>
         </is>
       </c>
     </row>
@@ -1970,12 +1970,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>PARTIDO EVOLUCION POLITICA</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -1985,12 +1985,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>UNION DEMOCRATA INDEPENDIENTE</t>
+          <t>PARTIDO ECOLOGISTA VERDE</t>
         </is>
       </c>
     </row>
@@ -2000,12 +2000,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>INDEPENDIENTES</t>
+          <t>SOMOS AYSEN</t>
         </is>
       </c>
     </row>
@@ -2015,12 +2015,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>PARTIDO REGIONALISTA DE MAGALLANES</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2030,12 +2030,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>PARTIDO SOCIALISTA DE CHILE</t>
+          <t>PARTIDO POR LA DEMOCRACIA</t>
         </is>
       </c>
     </row>
@@ -2045,12 +2045,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>INDEPENDIENTES</t>
+          <t>PARTIDO SOCIALISTA DE CHILE</t>
         </is>
       </c>
     </row>
@@ -2060,12 +2060,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>PARTIDO POR LA DEMOCRACIA</t>
+          <t>PARTIDO DEMOCRATA CRISTIANO</t>
         </is>
       </c>
     </row>
@@ -2075,12 +2075,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>PARTIDO DEMOCRATA CRISTIANO</t>
+          <t>PARTIDO RADICAL SOCIALDEMOCRATA</t>
         </is>
       </c>
     </row>
@@ -2090,12 +2090,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>PARTIDO RADICAL SOCIALDEMOCRATA</t>
+          <t>MAS REGION</t>
         </is>
       </c>
     </row>
@@ -2105,12 +2105,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>PARTIDO IZQUIERDA CIUDADANA DE CHILE</t>
+          <t>PARTIDO COMUNISTA DE CHILE</t>
         </is>
       </c>
     </row>
@@ -2120,12 +2120,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>F</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>PARTIDO COMUNISTA DE CHILE</t>
+          <t>UNION DEMOCRATA INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2135,12 +2135,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>F</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>MAS REGION</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2150,12 +2150,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>PODER</t>
+          <t>RENOVACION NACIONAL</t>
         </is>
       </c>
     </row>
@@ -2165,12 +2165,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO REGIONALISTA INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2180,12 +2180,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>I</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>PARTIDO ECOLOGISTA VERDE</t>
+          <t>AMPLITUD</t>
         </is>
       </c>
     </row>
@@ -2195,12 +2195,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>I</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>SOMOS AYSEN</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2225,12 +2225,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>PARTIDO POR LA DEMOCRACIA</t>
+          <t>REVOLUCION DEMOCRATICA</t>
         </is>
       </c>
     </row>
@@ -2240,12 +2240,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>PARTIDO SOCIALISTA DE CHILE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2255,12 +2255,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>PARTIDO DEMOCRATA CRISTIANO</t>
+          <t>PARTIDO IGUALDAD</t>
         </is>
       </c>
     </row>
@@ -2270,12 +2270,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>PARTIDO RADICAL SOCIALDEMOCRATA</t>
+          <t>PARTIDO FRENTE POPULAR</t>
         </is>
       </c>
     </row>
@@ -2285,12 +2285,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>MAS REGION</t>
+          <t>FUERZA REGIONAL NORTE VERDE</t>
         </is>
       </c>
     </row>
@@ -2300,12 +2300,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>PARTIDO COMUNISTA DE CHILE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2315,12 +2315,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>UNION DEMOCRATA INDEPENDIENTE</t>
+          <t>DEMOCRACIA REGIONAL PATAGONICA</t>
         </is>
       </c>
     </row>
@@ -2330,12 +2330,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO PROGRESISTA</t>
         </is>
       </c>
     </row>
@@ -2345,12 +2345,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>RENOVACION NACIONAL</t>
+          <t>FRENTE REGIONAL Y POPULAR</t>
         </is>
       </c>
     </row>
@@ -2360,12 +2360,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>PARTIDO REGIONALISTA INDEPENDIENTE</t>
+          <t>WALLMAPUWEN</t>
         </is>
       </c>
     </row>
@@ -2375,12 +2375,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>AMPLITUD</t>
+          <t>PARTIDO HUMANISTA</t>
         </is>
       </c>
     </row>
@@ -2390,12 +2390,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO LIBERAL DE CHILE</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2420,12 +2420,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>REVOLUCION DEMOCRATICA</t>
+          <t>MOVIMIENTO INDEPENDIENTE REGIONALISTA AGRARIO Y SOCIAL</t>
         </is>
       </c>
     </row>
@@ -2435,12 +2435,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>UNIDOS RESULTA EN DEMOCRACIA</t>
         </is>
       </c>
     </row>
@@ -2450,12 +2450,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>R</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>PARTIDO IGUALDAD</t>
+          <t>UNION PATRIOTICA</t>
         </is>
       </c>
     </row>
@@ -2465,12 +2465,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>R</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>PARTIDO FRENTE POPULAR</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2480,22 +2480,22 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>FUERZA REGIONAL NORTE VERDE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>CANDIDATURA INDEPENDIENTE</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2506,161 +2506,161 @@
     </row>
     <row r="144">
       <c r="A144">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>DEMOCRACIA REGIONAL PATAGONICA</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>PARTIDO PROGRESISTA</t>
+          <t>PARTIDO POR LA DEMOCRACIA</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>FRENTE REGIONAL Y POPULAR</t>
+          <t>PARTIDO RADICAL DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>WALLMAPUWEN</t>
+          <t>PARTIDO SOCIALISTA DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>PARTIDO HUMANISTA</t>
+          <t>PARTIDO COMUNISTA DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>PARTIDO LIBERAL DE CHILE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>FEDERACION REGIONALISTA VERDE SOCIAL</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>XE</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>MOVIMIENTO INDEPENDIENTE REGIONALISTA AGRARIO Y SOCIAL</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>XE</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>UNIDOS RESULTA EN DEMOCRACIA</t>
+          <t>PARTIDO NACIONAL CIUDADANO</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>XO</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>UNION PATRIOTICA</t>
+          <t>PARTIDO REPUBLICANO DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>XO</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2671,22 +2671,32 @@
     </row>
     <row r="155">
       <c r="A155">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>XS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO LIBERAL DE CHILE</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>2016</v>
+        <v>2021</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>XS</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>CONVERGENCIA SOCIAL</t>
+        </is>
       </c>
     </row>
     <row r="157">
@@ -2695,12 +2705,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>CANDIDATURA INDEPENDIENTE</t>
+          <t>XS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>REVOLUCION DEMOCRATICA</t>
         </is>
       </c>
     </row>
@@ -2710,7 +2720,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>XS</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -2725,12 +2735,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>XS</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>PARTIDO POR LA DEMOCRACIA</t>
+          <t>COMUNES</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2750,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>XU</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>PARTIDO RADICAL DE CHILE</t>
+          <t>PARTIDO DEMOCRATA CRISTIANO</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2765,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>XU</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>PARTIDO SOCIALISTA DE CHILE</t>
+          <t>PARTIDO PROGRESISTA DE CHILE</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2780,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>XU</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>PARTIDO COMUNISTA DE CHILE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2795,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>XU</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>CIUDADANOS</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2810,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>FEDERACION REGIONALISTA VERDE SOCIAL</t>
+          <t>UNION DEMOCRATA INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2825,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>XE</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>RENOVACION NACIONAL</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2840,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>XE</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>PARTIDO NACIONAL CIUDADANO</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2855,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>XO</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>PARTIDO REPUBLICANO DE CHILE</t>
+          <t>EVOLUCION POLITICA</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2870,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>XO</t>
+          <t>XX</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO REGIONALISTA INDEPENDIENTE DEMOCRATA</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2885,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>XY</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>PARTIDO LIBERAL DE CHILE</t>
+          <t>IGUALDAD</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2900,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>XY</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>CONVERGENCIA SOCIAL</t>
+          <t>PARTIDO HUMANISTA</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2915,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>XY</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>REVOLUCION DEMOCRATICA</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2930,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>XZ</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>PARTIDO ECOLOGISTA VERDE</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2945,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>XS</t>
+          <t>XZ</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>COMUNES</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2960,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>XU</t>
+          <t>YC</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>PARTIDO DEMOCRATA CRISTIANO</t>
+          <t>PARTIDO CONSERVADOR CRISTIANO</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2975,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>XU</t>
+          <t>YC</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>PARTIDO PROGRESISTA DE CHILE</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2990,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>XU</t>
+          <t>YG</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>NUEVO TIEMPO</t>
         </is>
       </c>
     </row>
@@ -2995,220 +3005,10 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>XU</t>
+          <t>ZB</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
-        <is>
-          <t>CIUDADANOS</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178">
-        <v>2021</v>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>XX</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>UNION DEMOCRATA INDEPENDIENTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179">
-        <v>2021</v>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>XX</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>RENOVACION NACIONAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180">
-        <v>2021</v>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>XX</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>INDEPENDIENTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181">
-        <v>2021</v>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>XX</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>EVOLUCION POLITICA</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182">
-        <v>2021</v>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>XX</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>PARTIDO REGIONALISTA INDEPENDIENTE DEMOCRATA</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183">
-        <v>2021</v>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>XY</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>IGUALDAD</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184">
-        <v>2021</v>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>XY</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>PARTIDO HUMANISTA</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185">
-        <v>2021</v>
-      </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>XY</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>INDEPENDIENTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186">
-        <v>2021</v>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>XZ</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>PARTIDO ECOLOGISTA VERDE</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187">
-        <v>2021</v>
-      </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>XZ</t>
-        </is>
-      </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>INDEPENDIENTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188">
-        <v>2021</v>
-      </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>YC</t>
-        </is>
-      </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>PARTIDO CONSERVADOR CRISTIANO</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189">
-        <v>2021</v>
-      </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>YC</t>
-        </is>
-      </c>
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>INDEPENDIENTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190">
-        <v>2021</v>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>YG</t>
-        </is>
-      </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>NUEVO TIEMPO</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191">
-        <v>2021</v>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>ZB</t>
-        </is>
-      </c>
-      <c r="C191" t="inlineStr">
         <is>
           <t>UNION PATRIOTICA</t>
         </is>

</xml_diff>